<commit_message>
Prevented addition of thermo information if path_mdf from pickaxe_thermodynamics returned None for mdf. Processed expansions for 240311 bottle pickaxe checkin
</commit_message>
<xml_diff>
--- a/artifacts/pwy_xls/ccm_v0_to_mvacid_gen_3_tan_sample_1_n_samples_1000.xlsx
+++ b/artifacts/pwy_xls/ccm_v0_to_mvacid_gen_3_tan_sample_1_n_samples_1000.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,6 +434,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>starter</t>
@@ -451,28 +456,43 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>mcs</t>
+          <t>pwy_ave_mcs</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>uniprot_1</t>
+          <t>mcs_rxn_1</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>uniprot_2</t>
+          <t>mcs_rxn_2</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>uniprot_3</t>
+          <t>mcs_rxn_3</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>uniprot_rxn_1</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>uniprot_rxn_2</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>uniprot_rxn_3</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -485,24 +505,33 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>30.21155927414979</v>
+        <v>37.58993642927125</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4529085129265492</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">R02243: [] | ACONITATE-DECARBOXYLASE-RXN_reverse: [B3IUN8, P54987, Q0C8L3] | </t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">RXN-863_reverse: [O87942, O87943, O87944, Q8VPT6, Q8VPT8] | R05598: [] | 4.1.99.11_13: [] | </t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">RXN-16543_reverse: [] | </t>
+        <v>0.6044071669071669</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.3839285714285714</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.7626262626262625</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Q0C8L3, P54987, B3IUN8</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>O87943, O87942, O87944</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Q5PDP3, Q989E7, Q3A133, Q9A5V1, P62456, Q02136, Q57MS3, Q606Q2, Q8XV79, Q46WL2, Q2P3K3, Q5LL27, Q82AA6, Q8EFB1, Q5WDH8, Q8ESR8, P16245, P62458, Q8YSM8, Q313T7, Q8YWL4, Q5QWP8, Q3Z878, P60862, Q4JW59, Q2RGV8, Q39K91, Q8P9P2, Q5ZW87, A0A0J9X7D2, Q97KI2, Q9K6Z2, P06988, Q47XB8, Q8PLG9, Q3MEV7, Q6D411, O34651, Q5V574, A1BPP9, Q722Y3, P60859, Q9PBC5, Q30TA4, Q8TXG3, P24226, Q7V5N9, Q92S26, Q9RQ88, Q5F7D8, Q8ZFX5, Q7VFF5, Q5HKN8, Q47AL5, P62457, Q39YP7, Q9JTH9, Q8ZY17, Q7NL02, O33775, Q6FEC8, Q323J2, Q5FS83, Q8R882, Q8F393, P62460, Q7M8K9, Q9HPW5, B0SS41, B0S9F2, Q65EF9, Q62GD9, Q5SKC1, Q3J7H1, Q4A044, Q63DX2, Q2YAU5, Q8D8Q0, Q318Q4, Q46J19, Q8G2R2, Q3AD53, Q6G5Z7, Q7WDY4, Q9P777, Q5E638, Q4FNE2, Q845V3, Q7VQX0, Q5KVC6, Q8G4S9, Q4QN74, Q8GKZ1, Q9ZHE6, Q3ICF0, Q3Z0G5, Q3J079, Q58851, O59626, Q48EC9, P44001, P63954, Q7W2Y4, P73058, Q9RSI4, Q87QL1, Q8X8T3, O26327, Q3ZXL7, Q81G06, Q8GDP4, P60861, Q4ZNV9, Q7V004, Q6HLE7, Q9RQ85, P18786, Q8DGR2, Q3B5E3, Q65RB1, P63953, Q8Z5K0, Q5X5W9, Q82W26, Q8UHX1, P9WNW8, Q5WX91, P60858, Q7VA26, Q8Y9G1, Q5HCL9, Q6GDC6, Q9CLM4, Q8ABA9, Q9C5U8, P59397, Q4J8I8, P10370, Q3SW26, Q5YYQ0, Q6A8L5, Q5MZ26, Q6AE76, Q8FG52, Q7U8K7, Q9L6I1, P63951, Q3JMZ6, Q7MLS6, Q9JYH8, Q8FNZ0, Q47QS9, Q3BUF7, Q4UU40, Q9RH05, Q3M5D3, Q7P0F6, Q8NNT5, Q31GY9, Q8DTQ7, Q492K3, Q2YZB4, Q57F99, Q81T62, P28736, Q2YPB8, Q5LAZ8, P9WNW9, P59398, P59400, O66976, P60860, P63952, O30027, Q5HSJ3, Q2RQM7, Q9HVW9, P62459, Q8PZR8, P59399, Q87C29, Q9F854, Q87WV5, Q9CC57, Q5P790, Q3AR25, Q8YF59, Q465R4, P59401, Q9X0D1, Q7VSZ1, Q7UX39, Q3SI67, Q63Q86, Q66C49, Q92E84, P57201, Q5H0L1, Q5JFR5, Q8CQ95, Q5NAY4, Q9PM77, Q970Y9, Q4FQF8, Q8TL41, Q6ANR3, Q3KHZ2, Q64RE7, Q6KZD1, Q9RQ82, Q8KEY6, Q67KH6, Q4KI73, Q32EE9</t>
         </is>
       </c>
     </row>
@@ -521,24 +550,33 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>37.58993642927175</v>
+        <v>30.21155927414955</v>
       </c>
       <c r="E3" t="n">
-        <v>0.4222189789926256</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">RXN0-1382: [A1ADQ1, A4YXN2, A5EGD7, A7ZPI2, A8A2M8, B1IX88, B1LMH0, B1X9P6, B2TWX3, B3QBS6, B5YYX4, B6I6S5, B6JE29, B7LBS7, B7M6P3, B7MH34, B7MY33, B7N5X4, B7NPQ8, B7UG84, C4ZVR1, O06644, O87838, P69902, P69903, Q07Q82, Q0TF87, Q139H7, Q1R8Z2, Q217M3, Q2IUI7, Q31Y97, Q32DG9, Q3YZF6, Q6N8F8, Q82M40, Q89QH2, Q8FFE8, Q8XBR7] | R07290: [] | 2.8.3.16_1: [] | 2.8.3.9_14: [] | </t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">RXN-863_reverse: [O87942, O87943, O87944, Q8VPT6, Q8VPT8] | R05598: [] | 4.1.99.11_13: [] | </t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">RXN-16543_reverse: [] | </t>
+        <v>0.4688516113516113</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.3839285714285714</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.7626262626262625</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Q89QH2, A4YXN2, B3QBS6, Q8XBR7, B7M6P3, A4G242, A5EGD7, Q46S66, Q2IUI7, B1X9P6, Q31Y97, Q6N8F8, B1IX88, A7ZPI2, B1LMH0, Q217M3, Q46S72, A4G241, Q8FFE8, B6JE29, B7NPQ8, C4ZVR1, A7ICK2, B7UG84, Q0TF87, Q82M40, A6T0J2, B2TWX3, Q0K0H8, A9X6P7, O87838, Q3YZF6, B5YYX4, P69902, Q07Q82, Q1R8Z2, B6I6S5, A8A2M8, Q13RQ4, B7LBS7, P69903, O06644, B7MH34, Q32DG9, B7MY33, A1ADQ1, B7N5X4, Q139H7</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>O87943, O87942, O87944</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Q5PDP3, Q989E7, Q3A133, Q9A5V1, P62456, Q02136, Q57MS3, Q606Q2, Q8XV79, Q46WL2, Q2P3K3, Q5LL27, Q82AA6, Q8EFB1, Q5WDH8, Q8ESR8, P16245, P62458, Q8YSM8, Q313T7, Q8YWL4, Q5QWP8, Q3Z878, P60862, Q4JW59, Q2RGV8, Q39K91, Q8P9P2, Q5ZW87, A0A0J9X7D2, Q97KI2, Q9K6Z2, P06988, Q47XB8, Q8PLG9, Q3MEV7, Q6D411, O34651, Q5V574, A1BPP9, Q722Y3, P60859, Q9PBC5, Q30TA4, Q8TXG3, P24226, Q7V5N9, Q92S26, Q9RQ88, Q5F7D8, Q8ZFX5, Q7VFF5, Q5HKN8, Q47AL5, P62457, Q39YP7, Q9JTH9, Q8ZY17, Q7NL02, O33775, Q6FEC8, Q323J2, Q5FS83, Q8R882, Q8F393, P62460, Q7M8K9, Q9HPW5, B0SS41, B0S9F2, Q65EF9, Q62GD9, Q5SKC1, Q3J7H1, Q4A044, Q63DX2, Q2YAU5, Q8D8Q0, Q318Q4, Q46J19, Q8G2R2, Q3AD53, Q6G5Z7, Q7WDY4, Q9P777, Q5E638, Q4FNE2, Q845V3, Q7VQX0, Q5KVC6, Q8G4S9, Q4QN74, Q8GKZ1, Q9ZHE6, Q3ICF0, Q3Z0G5, Q3J079, Q58851, O59626, Q48EC9, P44001, P63954, Q7W2Y4, P73058, Q9RSI4, Q87QL1, Q8X8T3, O26327, Q3ZXL7, Q81G06, Q8GDP4, P60861, Q4ZNV9, Q7V004, Q6HLE7, Q9RQ85, P18786, Q8DGR2, Q3B5E3, Q65RB1, P63953, Q8Z5K0, Q5X5W9, Q82W26, Q8UHX1, P9WNW8, Q5WX91, P60858, Q7VA26, Q8Y9G1, Q5HCL9, Q6GDC6, Q9CLM4, Q8ABA9, Q9C5U8, P59397, Q4J8I8, P10370, Q3SW26, Q5YYQ0, Q6A8L5, Q5MZ26, Q6AE76, Q8FG52, Q7U8K7, Q9L6I1, P63951, Q3JMZ6, Q7MLS6, Q9JYH8, Q8FNZ0, Q47QS9, Q3BUF7, Q4UU40, Q9RH05, Q3M5D3, Q7P0F6, Q8NNT5, Q31GY9, Q8DTQ7, Q492K3, Q2YZB4, Q57F99, Q81T62, P28736, Q2YPB8, Q5LAZ8, P9WNW9, P59398, P59400, O66976, P60860, P63952, O30027, Q5HSJ3, Q2RQM7, Q9HVW9, P62459, Q8PZR8, P59399, Q87C29, Q9F854, Q87WV5, Q9CC57, Q5P790, Q3AR25, Q8YF59, Q465R4, P59401, Q9X0D1, Q7VSZ1, Q7UX39, Q3SI67, Q63Q86, Q66C49, Q92E84, P57201, Q5H0L1, Q5JFR5, Q8CQ95, Q5NAY4, Q9PM77, Q970Y9, Q4FQF8, Q8TL41, Q6ANR3, Q3KHZ2, Q64RE7, Q6KZD1, Q9RQ82, Q8KEY6, Q67KH6, Q4KI73, Q32EE9</t>
         </is>
       </c>
     </row>

</xml_diff>